<commit_message>
Atualização automática de SAO_SEPE.xlsx
</commit_message>
<xml_diff>
--- a/SAO_SEPE.xlsx
+++ b/SAO_SEPE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B9B1120-B837-4F18-9958-B5E99D78F111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{23382675-6CA3-4667-825A-A22CBFA164D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1294,7 +1294,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{CE3EC9A3-CA09-44DA-83AD-391DD20A94F6}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{D4AD9C79-F68E-48A7-9E77-00E1DC3D55AB}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1324,10 +1324,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1AE76C5-2F77-4D0C-967B-F10ECA9D8658}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4A825A3-9ADC-42C4-B129-275EFEB92A7C}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1365,7 +1365,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{156D7A49-B596-46CF-AB04-FADA58961093}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{636B5350-7F9E-4BC5-9B07-B280B8928D9E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1428,7 +1428,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCA802FB-8DDF-4C02-B1BD-63C5FDC31A46}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A04D82C8-B0FE-4FF7-8784-859560ACDD59}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1447,7 +1447,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11281A7F-3E14-338C-FD6F-AB292317B696}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A86A184A-F6EE-CA89-86A6-D943B54037BC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1496,7 +1496,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B62D8E35-1D3A-EE3A-C3BB-F3B9E36540B9}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFE868ED-02C0-3A4A-06C2-7A2B87C88323}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1515,7 +1515,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5902A338-5D11-1D1C-EBBA-A3931CFD79CD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAFB0EA2-739D-C579-FE16-101D27A23A91}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1546,7 +1546,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{483C53A3-A57C-8400-D53E-6AED6271720F}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B5FB236-17D9-C50C-3A3D-33C5321D0533}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1577,7 +1577,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{806A643B-1375-9A66-AF58-0BD4A1934310}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8F975FB-D42F-8932-F1A8-8ADDEC3E2008}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1620,7 +1620,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F541A4C-73C6-4BBC-A5BC-85A29C00AF2B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1A9CADF-CB4D-42AA-81E6-2E41859398A3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1658,7 +1658,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26D53246-88E8-4870-8729-C2D2470294A4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A05E2E9-4CFD-4D46-B875-E8EE0A41E557}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1701,7 +1701,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{094C6C28-810D-4D36-91B3-D853574FEF00}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99FAE3C8-E624-482D-9E60-FC83437800C6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2014,7 +2014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5674B88-0518-4B3A-B5F1-3C8DC3F4C94C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AFF733E-8C72-46A8-AC9D-8DDA93D723C2}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>